<commit_message>
change font size for 100%
</commit_message>
<xml_diff>
--- a/your game name here final.xlsx
+++ b/your game name here final.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://instituteoftechnol663-my.sharepoint.com/personal/lowep_itcarlow_ie/Documents/game design/Labs 23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pete\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{092A1A6A-36D4-4DA5-84E8-017E00EC08D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDFF27F7-F1BA-4C73-B0CF-AE8E2C396A19}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE96A8E-7595-4651-A730-EDF9F0217048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="e3XNt+Y+1D3+D24i3JY7ZfvaUeJ+Ficv5JqUYqK3GxA1BYB7FHhPYhxuoVdsKOXJwPbSFyACJvbToUlhxA/0dg==" workbookSaltValue="bwSytUchgVbQ5tn7OpDLYQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B114BF61-C9F1-47F8-B51B-C5362F104DFD}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B114BF61-C9F1-47F8-B51B-C5362F104DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,7 +272,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -586,20 +586,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1AE6D3-2084-479B-AB85-13952D070B1F}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" customWidth="1"/>
     <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="11" width="4.28515625" customWidth="1"/>
+    <col min="8" max="11" width="5.42578125" customWidth="1"/>
     <col min="14" max="17" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C2">
         <f>SUM(C4:C23)</f>
         <v>50</v>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -694,7 +694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1204,18 +1204,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rE/jSGPP/aE6BlwRnSXSsYHhuwabxFVXqnu4SvramUzBJawLpNMSuQYXx5z7Qe+md3Abu1waghaaJ4M6GzWMXg==" saltValue="oReG4eohyeC2eEQq0YmyfQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nYrsWWHhavrBlv7BI4ZdmwNRmp+fCUTesnAxySaJ5kOHahb9JRseiPmf8wZ+CLRgixEjOQtsbaAN1qHR4nJSsw==" saltValue="CcLmag1E9yzeijRNy8rXAw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="B15:B18" name="Range2"/>
     <protectedRange sqref="H4:K13" name="Range1"/>

</xml_diff>